<commit_message>
added redo of OHE table
</commit_message>
<xml_diff>
--- a/assets/2023-07-28_Spreadsheet.xlsx
+++ b/assets/2023-07-28_Spreadsheet.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="I_have_a_fever" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="word-embed-private-main" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Table 1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet1_2" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
   <si>
     <t xml:space="preserve">unique word</t>
   </si>
@@ -256,16 +258,275 @@
   </si>
   <si>
     <t xml:space="preserve">'to'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doc 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doc 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doc 3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF494949"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Vocabulary </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF5B5B5B"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">size </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF494949"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(N) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF6B6B6B"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF494949"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">14</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF494949"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color rgb="FF494949"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">..</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF494949"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color rgb="FF494949"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="21"/>
+        <color rgb="FF5B5B5B"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF494949"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="21"/>
+        <color rgb="FF5B5B5B"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF494949"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">b</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="12"/>
+        <color rgb="FF494949"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF494949"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">o</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF282828"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="21"/>
+        <color rgb="FF494949"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF282828"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="21"/>
+        <color rgb="FF494949"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF494949"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">One</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF6B6B6B"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF494949"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">hot vector</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Length of vector = 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vocabulary size (N) =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One-hot vector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="###0;###0"/>
+    <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -331,6 +592,145 @@
       <color rgb="FF000000"/>
       <name val="Calibri "/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF494949"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF5B5B5B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF6B6B6B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF494949"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF494949"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF494949"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color rgb="FF494949"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF5B5B5B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF494949"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF494949"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="21"/>
+      <color rgb="FF5B5B5B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF494949"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF494949"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF494949"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF282828"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="21"/>
+      <color rgb="FF494949"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Default Metrics Font"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -344,7 +744,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4472C4"/>
-        <bgColor rgb="FF666699"/>
+        <bgColor rgb="FF6B6B6B"/>
       </patternFill>
     </fill>
     <fill>
@@ -366,7 +766,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -379,6 +779,40 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin">
+        <color rgb="FF282828"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF282828"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF282828"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="medium"/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -407,7 +841,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,26 +886,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,6 +904,78 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -510,7 +1004,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF5B5B5B"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -541,16 +1035,16 @@
       <rgbColor rgb="FFFFBF00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF6B6B6B"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF282828"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF494949"/>
+      <rgbColor rgb="FF3A3A3A"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -981,7 +1475,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1041,7 +1535,7 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1058,7 +1552,7 @@
       <c r="B1" s="10"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1066,23 +1560,23 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -1090,7 +1584,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1098,7 +1592,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -1106,18 +1600,18 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="13" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1136,59 +1630,1101 @@
       <c r="B12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="14" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="15" t="s">
         <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.40625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="9.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="9.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="1.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="32.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B13" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" s="19"/>
+      <c r="N16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="18"/>
+      <c r="N17" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="4.33"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="32"/>
+      <c r="C8" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" s="32"/>
+      <c r="C9" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" s="32"/>
+      <c r="C10" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" s="32"/>
+      <c r="C14" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="32"/>
+      <c r="G16" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="32"/>
+      <c r="E18" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B20" s="32"/>
+      <c r="C20" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="30" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>